<commit_message>
sign up functionality completed
</commit_message>
<xml_diff>
--- a/ProjectData/Docs/API_Details.xlsx
+++ b/ProjectData/Docs/API_Details.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Sr No.</t>
   </si>
@@ -61,7 +61,38 @@
 }</t>
   </si>
   <si>
-    <t>in-progress</t>
+    <t>signup</t>
+  </si>
+  <si>
+    <t>api/signup</t>
+  </si>
+  <si>
+    <t>{
+    "firstName":$scope.firstName,
+    "lastName":$scope.lastName,
+    "userEmail":$scope.userEmail,
+    "mobileNumber":$scope.mobileNumber,
+    "country":$scope.selectedCountry,
+    "zipcode":$scope.zipcode
+}</t>
+  </si>
+  <si>
+    <t>done</t>
+  </si>
+  <si>
+    <t>backend pending</t>
+  </si>
+  <si>
+    <t>{
+   "statusCode":200,
+   "signedup":true,
+   "message":{
+     "title":"",
+     "messageText":""
+   },
+   "data":{ 
+    }
+}</t>
   </si>
 </sst>
 </file>
@@ -85,7 +116,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -172,11 +203,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -202,26 +242,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="11">
     <dxf>
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
+      <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
         <right style="thin">
           <color indexed="64"/>
         </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -255,11 +299,60 @@
       </border>
     </dxf>
     <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
         <right style="thin">
           <color indexed="64"/>
         </right>
@@ -290,8 +383,7 @@
       </border>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
+      <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -307,21 +399,14 @@
       </border>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
+      <border>
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
       </border>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
@@ -337,48 +422,6 @@
         <horizontal style="thin">
           <color indexed="64"/>
         </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
       </border>
     </dxf>
   </dxfs>
@@ -392,14 +435,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="API_Details" displayName="API_Details" ref="C5:H6" headerRowDxfId="8" totalsRowDxfId="7" headerRowBorderDxfId="9" tableBorderDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="API_Details" displayName="API_Details" ref="C5:H7" headerRowDxfId="10" totalsRowDxfId="7" headerRowBorderDxfId="9" tableBorderDxfId="8">
   <tableColumns count="6">
     <tableColumn id="4" name="Sr No." dataDxfId="6"/>
     <tableColumn id="3" name="Screen" dataDxfId="5"/>
-    <tableColumn id="2" name="Url" dataDxfId="3"/>
-    <tableColumn id="1" name="Request" totalsRowFunction="count" dataDxfId="2"/>
-    <tableColumn id="5" name="Response" dataDxfId="0"/>
-    <tableColumn id="6" name="Integration Status" dataDxfId="1" totalsRowDxfId="4"/>
+    <tableColumn id="2" name="Url" dataDxfId="4"/>
+    <tableColumn id="1" name="Request" totalsRowFunction="count" dataDxfId="3"/>
+    <tableColumn id="5" name="Response" dataDxfId="2"/>
+    <tableColumn id="6" name="Integration Status" dataDxfId="1" totalsRowDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -692,10 +735,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C5:H6"/>
+  <dimension ref="C5:H7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -746,18 +789,39 @@
         <v>9</v>
       </c>
       <c r="H6" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="3:8" ht="150" x14ac:dyDescent="0.25">
+      <c r="C7" s="4">
+        <v>2</v>
+      </c>
+      <c r="D7" s="5" t="s">
         <v>10</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="H7" s="9" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="H6">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="H6:H7">
       <formula1>"in-progress,done,not-started,UI pending,backend pending"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>